<commit_message>
Add standard errors by running ablation 30 times
</commit_message>
<xml_diff>
--- a/results/real_regression_insurance.xlsx
+++ b/results/real_regression_insurance.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arushi Jain\MIT Dropbox\Arushi Jain\FairAI\results\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1347F3-08E8-45F8-9355-D21FA33E92E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Protected_Feature</t>
   </si>
@@ -22,30 +28,9 @@
     <t>Protected_Class</t>
   </si>
   <si>
-    <t>weighted_average_target</t>
-  </si>
-  <si>
-    <t>weighted_otheravg_target</t>
-  </si>
-  <si>
-    <t>weighted_Fairness_target</t>
-  </si>
-  <si>
-    <t>weighted_average_pred</t>
-  </si>
-  <si>
-    <t>weighted_otheravg_pred</t>
-  </si>
-  <si>
-    <t>weighted_Fairness_pred</t>
-  </si>
-  <si>
     <t>count</t>
   </si>
   <si>
-    <t>dataset</t>
-  </si>
-  <si>
     <t>region</t>
   </si>
   <si>
@@ -79,14 +64,17 @@
     <t>yes</t>
   </si>
   <si>
-    <t>Insurance</t>
+    <t>Fairness_target</t>
+  </si>
+  <si>
+    <t>Fairness_pred</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,13 +137,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -193,7 +189,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -227,6 +223,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -261,9 +258,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -436,14 +434,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -451,284 +451,149 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>0.97120716908440197</v>
+      </c>
+      <c r="D2">
+        <v>0.9239137191383624</v>
+      </c>
+      <c r="E2">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>0.97590549968131657</v>
+      </c>
+      <c r="D3">
+        <v>0.95490996940646433</v>
+      </c>
+      <c r="E3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>0.97263915442447624</v>
+      </c>
+      <c r="D4">
+        <v>0.89358359928046882</v>
+      </c>
+      <c r="E4">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>0.98055575017457053</v>
+      </c>
+      <c r="D5">
+        <v>0.95780895578652869</v>
+      </c>
+      <c r="E5">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>0.97410348663068802</v>
+      </c>
+      <c r="D6">
+        <v>0.96282472149664089</v>
+      </c>
+      <c r="E6">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>0.96881175814991172</v>
+      </c>
+      <c r="D7">
+        <v>0.96448142155844319</v>
+      </c>
+      <c r="E7">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>0.22716653936679801</v>
+      </c>
+      <c r="D8">
+        <v>0.11516152419090669</v>
+      </c>
+      <c r="E8">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
         <v>13</v>
       </c>
-      <c r="C2">
-        <v>13406.3845163858</v>
-      </c>
-      <c r="D2">
-        <v>13552.18066525618</v>
-      </c>
-      <c r="E2">
-        <v>0.971207169084402</v>
-      </c>
-      <c r="F2">
-        <v>12764.01644468137</v>
-      </c>
-      <c r="G2">
-        <v>13748.92239028916</v>
-      </c>
-      <c r="H2">
-        <v>0.9239137191383624</v>
-      </c>
-      <c r="I2">
-        <v>324</v>
-      </c>
-      <c r="J2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3">
-        <v>12417.57537396923</v>
-      </c>
-      <c r="D3">
-        <v>12293.14098092523</v>
-      </c>
-      <c r="E3">
-        <v>0.9759054996813166</v>
-      </c>
-      <c r="F3">
-        <v>12810.60590334252</v>
-      </c>
-      <c r="G3">
-        <v>13329.97981085275</v>
-      </c>
-      <c r="H3">
-        <v>0.9549099694064643</v>
-      </c>
-      <c r="I3">
-        <v>325</v>
-      </c>
-      <c r="J3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4">
-        <v>14735.41143760989</v>
-      </c>
-      <c r="D4">
-        <v>14557.68139329294</v>
-      </c>
-      <c r="E4">
-        <v>0.9726391544244762</v>
-      </c>
-      <c r="F4">
-        <v>14075.71465381813</v>
-      </c>
-      <c r="G4">
-        <v>12693.07229637429</v>
-      </c>
-      <c r="H4">
-        <v>0.8935835992804688</v>
-      </c>
-      <c r="I4">
-        <v>364</v>
-      </c>
-      <c r="J4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5">
-        <v>12346.93737729231</v>
-      </c>
-      <c r="D5">
-        <v>12512.66336136486</v>
-      </c>
-      <c r="E5">
-        <v>0.9805557501745705</v>
-      </c>
-      <c r="F5">
-        <v>13333.15880032653</v>
-      </c>
-      <c r="G5">
-        <v>13320.17180569742</v>
-      </c>
-      <c r="H5">
-        <v>0.9578089557865287</v>
-      </c>
-      <c r="I5">
-        <v>325</v>
-      </c>
-      <c r="J5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6">
-        <v>12569.57884383535</v>
-      </c>
-      <c r="D6">
-        <v>12555.81603828952</v>
-      </c>
-      <c r="E6">
-        <v>0.974103486630688</v>
-      </c>
-      <c r="F6">
-        <v>13235.25509783326</v>
-      </c>
-      <c r="G6">
-        <v>13433.92867888657</v>
-      </c>
-      <c r="H6">
-        <v>0.9628247214966409</v>
-      </c>
-      <c r="I6">
-        <v>662</v>
-      </c>
-      <c r="J6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7">
-        <v>13956.75117772189</v>
-      </c>
-      <c r="D7">
-        <v>14020.97924009847</v>
-      </c>
-      <c r="E7">
-        <v>0.9688117581499117</v>
-      </c>
-      <c r="F7">
-        <v>13304.86111833341</v>
-      </c>
-      <c r="G7">
-        <v>13151.29029171568</v>
-      </c>
-      <c r="H7">
-        <v>0.9644814215584432</v>
-      </c>
-      <c r="I7">
-        <v>676</v>
-      </c>
-      <c r="J7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8">
-        <v>8434.268297856204</v>
-      </c>
-      <c r="D8">
-        <v>4348.661601909075</v>
-      </c>
-      <c r="E8">
-        <v>0.227166539366798</v>
-      </c>
-      <c r="F8">
-        <v>13306.81639415181</v>
-      </c>
-      <c r="G8">
-        <v>1849.276158783805</v>
-      </c>
-      <c r="H8">
-        <v>0.1151615241909067</v>
-      </c>
-      <c r="I8">
-        <v>1064</v>
-      </c>
-      <c r="J8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
       <c r="C9">
-        <v>32050.23183153285</v>
+        <v>0.88936160845936651</v>
       </c>
       <c r="D9">
-        <v>28216.71176767616</v>
+        <v>0.76581994770009987</v>
       </c>
       <c r="E9">
-        <v>0.8893616084593665</v>
-      </c>
-      <c r="F9">
-        <v>13129.09615832654</v>
-      </c>
-      <c r="G9">
-        <v>17167.99303607987</v>
-      </c>
-      <c r="H9">
-        <v>0.7658199477000999</v>
-      </c>
-      <c r="I9">
         <v>274</v>
-      </c>
-      <c r="J9" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>